<commit_message>
Removed item charge type. All items use the same charge source. Moved all trinket type cards under item type.
</commit_message>
<xml_diff>
--- a/sheet/GearCardData.xlsx
+++ b/sheet/GearCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF677911-7F88-480D-BD0D-6906D2BF78DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FDC919-5459-4E84-A651-6F47AEDABDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,39 +35,13 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tags</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>待办清单</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,10 +53,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tagsEn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Extra pocket</t>
   </si>
   <si>
@@ -107,9 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Can be used when using another artifact: If you need to cost ammo, you can consume scrolls instead. And vice versa. (You can not convert part of the cost. For example, an artifact costing 2 scroll cannot be changed to cost 1 scroll and 1 ammo).</t>
-  </si>
-  <si>
     <t>Can be used when setting cards into Battlefield: You can set card on Opponent's Side.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,10 +89,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Magibullet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>战利品区容量加1。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -167,14 +130,6 @@
   </si>
   <si>
     <t>imageFile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>炼药锅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔弹射手</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -192,51 +147,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>被动</t>
-  </si>
-  <si>
-    <t>被动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">长休时，可以额外消耗1时间。&lt;br&gt;
 休息时，每消耗1时间，额外抽1张牌。
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>万能电池</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可以无视道具牌的标签使用战利品牌充能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用标签包含“食物”的道具牌后，可以选1张标签包含“药水”的道具牌充1能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用标签包含“卷轴”的道具牌后，可以选1张标签包含“弹药”的道具牌充1能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>魔瓶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用标签包含“药水”的道具牌后，可以选1张标签包含“卷轴”的道具牌充1能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>豌豆枪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用标签包含“弹药”的道具牌后，可以选1张标签包含“食物”的道具牌充1能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>向战场出牌时，可以将牌出在敌对侧。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -249,11 +165,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>王冠徽章</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"史莱姆"牌因效果进入房间区时，可以将其加入手牌。</t>
+    <t>捕梦网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以将未被选择的翻开的牌以任意顺序放回原牌堆顶或原牌堆底。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dream catcher</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -306,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -315,6 +235,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -596,312 +517,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="35.875" customWidth="1"/>
-    <col min="7" max="7" width="53.125" customWidth="1"/>
+    <col min="2" max="3" width="35.875" customWidth="1"/>
+    <col min="5" max="5" width="53.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="str" cm="1">
-        <f t="array" ref="F2">_xlfn.SWITCH(B2, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="str" cm="1">
-        <f t="array" ref="F3">_xlfn.SWITCH(B3, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="str" cm="1">
-        <f t="array" ref="F8">_xlfn.SWITCH(B8, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="str" cm="1">
-        <f t="array" ref="F11">_xlfn.SWITCH(B11, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="str" cm="1">
-        <f t="array" ref="F13">_xlfn.SWITCH(B13, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="str" cm="1">
-        <f t="array" ref="F14">_xlfn.SWITCH(B14, "药水", "Potion", "食物", "Food", "弹药", "Ammo", "卷轴", "Scroll", "")</f>
-        <v/>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>